<commit_message>
Feature reserva con fecha especifica
</commit_message>
<xml_diff>
--- a/src/test/resources/co.com.qr.capacitaciones.web/datadriver/reservar/Reserva.xlsx
+++ b/src/test/resources/co.com.qr.capacitaciones.web/datadriver/reservar/Reserva.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Codiguero_Automatizacion\src\test\resources\co.com.qr.capacitaciones.web\datadriver\reservar\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EQUIPO\Documents\capa\src\test\resources\co.com.qr.capacitaciones.web\datadriver\reservar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A80E7757-0942-4AE9-BE99-51700D3894AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8136" yWindow="6132" windowWidth="33372" windowHeight="20076" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="6504"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>origen</t>
   </si>
@@ -39,19 +38,22 @@
     <t>Cartagena</t>
   </si>
   <si>
-    <t>21</t>
-  </si>
-  <si>
     <t>fecha_inicial</t>
   </si>
   <si>
     <t>fecha_final</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -391,11 +393,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -414,10 +416,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -428,10 +430,10 @@
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
finalizacion feature reserva con fecha específica
</commit_message>
<xml_diff>
--- a/src/test/resources/co.com.qr.capacitaciones.web/datadriver/reservar/Reserva.xlsx
+++ b/src/test/resources/co.com.qr.capacitaciones.web/datadriver/reservar/Reserva.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="6504"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6510"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
     <t>17</t>
   </si>
   <si>
-    <t>5</t>
+    <t>11</t>
   </si>
 </sst>
 </file>
@@ -397,18 +397,18 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.109375" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -422,7 +422,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -436,7 +436,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>

</xml_diff>